<commit_message>
add term_paths, fix translation filter,
</commit_message>
<xml_diff>
--- a/database/imports/term_metas.xlsx
+++ b/database/imports/term_metas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\PHP\Laravel\LaravelOcadmin\laraocadmin10\httpdocs\database\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC7D536-0990-4476-8F3F-3AF90E7B3600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87022B7-CDAE-4E12-BAEC-1A548E337578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="term_metas" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="197">
   <si>
     <t>locale</t>
   </si>
@@ -581,9 +581,6 @@
     <t>Minivan</t>
   </si>
   <si>
-    <t>面包车</t>
-  </si>
-  <si>
     <t>貨車封閉式</t>
   </si>
   <si>
@@ -607,6 +604,58 @@
   </si>
   <si>
     <t>Cargo Van</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小客車</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.8L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.4L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.0L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.6L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.8L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.0L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5L</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.6L</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1200,8 +1249,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1559,11 +1611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F282"/>
+  <dimension ref="A1:F306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D253" sqref="D253:D267"/>
+      <pane ySplit="2" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F285" sqref="F285:G299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1571,7 +1623,7 @@
     <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
     <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1584,7 +1636,7 @@
       <c r="C1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1598,7 +1650,7 @@
       <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1612,7 +1664,7 @@
       <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1626,7 +1678,7 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1640,7 +1692,7 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1654,7 +1706,7 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1668,7 +1720,7 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1682,7 +1734,7 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1696,7 +1748,7 @@
       <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1710,7 +1762,7 @@
       <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1724,7 +1776,7 @@
       <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1738,7 +1790,7 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1752,7 +1804,7 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1766,7 +1818,7 @@
       <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1780,7 +1832,7 @@
       <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1794,7 +1846,7 @@
       <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1808,7 +1860,7 @@
       <c r="C17" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1822,7 +1874,7 @@
       <c r="C18" t="s">
         <v>36</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1836,7 +1888,7 @@
       <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1850,7 +1902,7 @@
       <c r="C20" t="s">
         <v>36</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1864,7 +1916,7 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1878,7 +1930,7 @@
       <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1892,7 +1944,7 @@
       <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1906,7 +1958,7 @@
       <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1920,7 +1972,7 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1934,7 +1986,7 @@
       <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1948,7 +2000,7 @@
       <c r="C27" t="s">
         <v>36</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1962,7 +2014,7 @@
       <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1976,7 +2028,7 @@
       <c r="C29" t="s">
         <v>36</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1990,7 +2042,7 @@
       <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2004,7 +2056,7 @@
       <c r="C31" t="s">
         <v>36</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2018,7 +2070,7 @@
       <c r="C32" t="s">
         <v>36</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2032,7 +2084,7 @@
       <c r="C33" t="s">
         <v>36</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2046,7 +2098,7 @@
       <c r="C34" t="s">
         <v>36</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2060,7 +2112,7 @@
       <c r="C35" t="s">
         <v>36</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2074,7 +2126,7 @@
       <c r="C36" t="s">
         <v>36</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2088,7 +2140,7 @@
       <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2102,7 +2154,7 @@
       <c r="C38" t="s">
         <v>36</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2116,7 +2168,7 @@
       <c r="C39" t="s">
         <v>36</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2130,7 +2182,7 @@
       <c r="C40" t="s">
         <v>36</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2144,7 +2196,7 @@
       <c r="C41" t="s">
         <v>36</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2158,7 +2210,7 @@
       <c r="C42" t="s">
         <v>36</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2172,7 +2224,7 @@
       <c r="C43" t="s">
         <v>36</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2186,7 +2238,7 @@
       <c r="C44" t="s">
         <v>36</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2200,7 +2252,7 @@
       <c r="C45" t="s">
         <v>36</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2214,7 +2266,7 @@
       <c r="C46" t="s">
         <v>36</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2228,7 +2280,7 @@
       <c r="C47" t="s">
         <v>36</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2242,7 +2294,7 @@
       <c r="C48" t="s">
         <v>36</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2256,7 +2308,7 @@
       <c r="C49" t="s">
         <v>36</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2270,7 +2322,7 @@
       <c r="C50" t="s">
         <v>36</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2284,7 +2336,7 @@
       <c r="C51" t="s">
         <v>36</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2298,7 +2350,7 @@
       <c r="C52" t="s">
         <v>36</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2312,7 +2364,7 @@
       <c r="C53" t="s">
         <v>36</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2326,7 +2378,7 @@
       <c r="C54" t="s">
         <v>36</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2340,7 +2392,7 @@
       <c r="C55" t="s">
         <v>36</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2354,7 +2406,7 @@
       <c r="C56" t="s">
         <v>36</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2368,7 +2420,7 @@
       <c r="C57" t="s">
         <v>36</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2382,7 +2434,7 @@
       <c r="C58" t="s">
         <v>36</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2396,7 +2448,7 @@
       <c r="C59" t="s">
         <v>36</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2410,7 +2462,7 @@
       <c r="C60" t="s">
         <v>36</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2424,7 +2476,7 @@
       <c r="C61" t="s">
         <v>36</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2438,7 +2490,7 @@
       <c r="C62" t="s">
         <v>36</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2452,7 +2504,7 @@
       <c r="C63" t="s">
         <v>36</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2466,7 +2518,7 @@
       <c r="C64" t="s">
         <v>36</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2480,7 +2532,7 @@
       <c r="C65" t="s">
         <v>36</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2494,7 +2546,7 @@
       <c r="C66" t="s">
         <v>36</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2508,7 +2560,7 @@
       <c r="C67" t="s">
         <v>36</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2522,7 +2574,7 @@
       <c r="C68" t="s">
         <v>36</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2536,7 +2588,7 @@
       <c r="C69" t="s">
         <v>36</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2550,7 +2602,7 @@
       <c r="C70" t="s">
         <v>36</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2564,7 +2616,7 @@
       <c r="C71" t="s">
         <v>36</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2578,7 +2630,7 @@
       <c r="C72" t="s">
         <v>36</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2592,7 +2644,7 @@
       <c r="C73" t="s">
         <v>36</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2606,7 +2658,7 @@
       <c r="C74" t="s">
         <v>36</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2620,7 +2672,7 @@
       <c r="C75" t="s">
         <v>36</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2634,7 +2686,7 @@
       <c r="C76" t="s">
         <v>36</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2648,7 +2700,7 @@
       <c r="C77" t="s">
         <v>36</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2662,7 +2714,7 @@
       <c r="C78" t="s">
         <v>36</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2676,7 +2728,7 @@
       <c r="C79" t="s">
         <v>36</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2690,7 +2742,7 @@
       <c r="C80" t="s">
         <v>36</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2704,7 +2756,7 @@
       <c r="C81" t="s">
         <v>36</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2718,7 +2770,7 @@
       <c r="C82" t="s">
         <v>36</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2732,7 +2784,7 @@
       <c r="C83" t="s">
         <v>36</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2746,7 +2798,7 @@
       <c r="C84" t="s">
         <v>36</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2760,7 +2812,7 @@
       <c r="C85" t="s">
         <v>36</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2774,7 +2826,7 @@
       <c r="C86" t="s">
         <v>36</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2788,7 +2840,7 @@
       <c r="C87" t="s">
         <v>36</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2802,7 +2854,7 @@
       <c r="C88" t="s">
         <v>36</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2816,7 +2868,7 @@
       <c r="C89" t="s">
         <v>36</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2830,7 +2882,7 @@
       <c r="C90" t="s">
         <v>36</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2844,7 +2896,7 @@
       <c r="C91" t="s">
         <v>36</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2858,7 +2910,7 @@
       <c r="C92" t="s">
         <v>36</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2872,7 +2924,7 @@
       <c r="C93" t="s">
         <v>36</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2886,7 +2938,7 @@
       <c r="C94" t="s">
         <v>36</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2900,7 +2952,7 @@
       <c r="C95" t="s">
         <v>36</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2914,7 +2966,7 @@
       <c r="C96" t="s">
         <v>36</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2928,7 +2980,7 @@
       <c r="C97" t="s">
         <v>36</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2942,7 +2994,7 @@
       <c r="C98" t="s">
         <v>36</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2956,7 +3008,7 @@
       <c r="C99" t="s">
         <v>36</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2970,7 +3022,7 @@
       <c r="C100" t="s">
         <v>36</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2984,7 +3036,7 @@
       <c r="C101" t="s">
         <v>36</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2998,7 +3050,7 @@
       <c r="C102" t="s">
         <v>36</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3012,7 +3064,7 @@
       <c r="C103" t="s">
         <v>36</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3026,7 +3078,7 @@
       <c r="C104" t="s">
         <v>36</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3040,7 +3092,7 @@
       <c r="C105" t="s">
         <v>36</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3054,7 +3106,7 @@
       <c r="C106" t="s">
         <v>36</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3068,7 +3120,7 @@
       <c r="C107" t="s">
         <v>36</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3082,7 +3134,7 @@
       <c r="C108" t="s">
         <v>36</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3096,7 +3148,7 @@
       <c r="C109" t="s">
         <v>36</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3110,7 +3162,7 @@
       <c r="C110" t="s">
         <v>36</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3124,7 +3176,7 @@
       <c r="C111" t="s">
         <v>36</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3138,7 +3190,7 @@
       <c r="C112" t="s">
         <v>36</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3152,7 +3204,7 @@
       <c r="C113" t="s">
         <v>36</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3166,7 +3218,7 @@
       <c r="C114" t="s">
         <v>36</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="1" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3180,7 +3232,7 @@
       <c r="C115" t="s">
         <v>36</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3194,7 +3246,7 @@
       <c r="C116" t="s">
         <v>36</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3208,7 +3260,7 @@
       <c r="C117" t="s">
         <v>36</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="1" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3222,7 +3274,7 @@
       <c r="C118" t="s">
         <v>36</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3236,7 +3288,7 @@
       <c r="C119" t="s">
         <v>36</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3250,7 +3302,7 @@
       <c r="C120" t="s">
         <v>36</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3264,7 +3316,7 @@
       <c r="C121" t="s">
         <v>36</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3278,7 +3330,7 @@
       <c r="C122" t="s">
         <v>36</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3292,7 +3344,7 @@
       <c r="C123" t="s">
         <v>36</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3306,7 +3358,7 @@
       <c r="C124" t="s">
         <v>36</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3320,7 +3372,7 @@
       <c r="C125" t="s">
         <v>36</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3334,7 +3386,7 @@
       <c r="C126" t="s">
         <v>36</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3348,7 +3400,7 @@
       <c r="C127" t="s">
         <v>36</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3362,7 +3414,7 @@
       <c r="C128" t="s">
         <v>36</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3376,7 +3428,7 @@
       <c r="C129" t="s">
         <v>36</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3390,7 +3442,7 @@
       <c r="C130" t="s">
         <v>36</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3404,7 +3456,7 @@
       <c r="C131" t="s">
         <v>36</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="1" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3418,7 +3470,7 @@
       <c r="C132" t="s">
         <v>36</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3432,7 +3484,7 @@
       <c r="C133" t="s">
         <v>36</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3446,7 +3498,7 @@
       <c r="C134" t="s">
         <v>36</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3460,7 +3512,7 @@
       <c r="C135" t="s">
         <v>36</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3474,7 +3526,7 @@
       <c r="C136" t="s">
         <v>36</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3488,7 +3540,7 @@
       <c r="C137" t="s">
         <v>36</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3502,7 +3554,7 @@
       <c r="C138" t="s">
         <v>36</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3516,7 +3568,7 @@
       <c r="C139" t="s">
         <v>36</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3530,7 +3582,7 @@
       <c r="C140" t="s">
         <v>36</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="1" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3544,7 +3596,7 @@
       <c r="C141" t="s">
         <v>36</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3558,7 +3610,7 @@
       <c r="C142" t="s">
         <v>36</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3572,7 +3624,7 @@
       <c r="C143" t="s">
         <v>36</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3586,7 +3638,7 @@
       <c r="C144" t="s">
         <v>36</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3600,7 +3652,7 @@
       <c r="C145" t="s">
         <v>36</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3614,7 +3666,7 @@
       <c r="C146" t="s">
         <v>36</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3628,7 +3680,7 @@
       <c r="C147" t="s">
         <v>36</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3642,7 +3694,7 @@
       <c r="C148" t="s">
         <v>36</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3656,7 +3708,7 @@
       <c r="C149" t="s">
         <v>36</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="1" t="s">
         <v>100</v>
       </c>
       <c r="E149">
@@ -3676,7 +3728,7 @@
       <c r="C150" t="s">
         <v>36</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E150">
@@ -3696,7 +3748,7 @@
       <c r="C151" t="s">
         <v>36</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E151">
@@ -3716,7 +3768,7 @@
       <c r="C152" t="s">
         <v>36</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="1" t="s">
         <v>103</v>
       </c>
       <c r="E152">
@@ -3736,7 +3788,7 @@
       <c r="C153" t="s">
         <v>36</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E153">
@@ -3756,7 +3808,7 @@
       <c r="C154" t="s">
         <v>36</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E154">
@@ -3776,7 +3828,7 @@
       <c r="C155" t="s">
         <v>36</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D155" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E155">
@@ -3796,7 +3848,7 @@
       <c r="C156" t="s">
         <v>36</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="1" t="s">
         <v>107</v>
       </c>
       <c r="E156">
@@ -3816,7 +3868,7 @@
       <c r="C157" t="s">
         <v>36</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157" s="1" t="s">
         <v>108</v>
       </c>
       <c r="E157">
@@ -3836,7 +3888,7 @@
       <c r="C158" t="s">
         <v>36</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="1" t="s">
         <v>109</v>
       </c>
       <c r="E158">
@@ -3856,7 +3908,7 @@
       <c r="C159" t="s">
         <v>36</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="1" t="s">
         <v>110</v>
       </c>
       <c r="E159">
@@ -3876,7 +3928,7 @@
       <c r="C160" t="s">
         <v>36</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D160" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E160">
@@ -3896,7 +3948,7 @@
       <c r="C161" t="s">
         <v>36</v>
       </c>
-      <c r="D161">
+      <c r="D161" s="1">
         <v>86</v>
       </c>
       <c r="E161">
@@ -3916,7 +3968,7 @@
       <c r="C162" t="s">
         <v>36</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="1" t="s">
         <v>112</v>
       </c>
       <c r="E162">
@@ -3936,7 +3988,7 @@
       <c r="C163" t="s">
         <v>36</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D163" s="1" t="s">
         <v>113</v>
       </c>
       <c r="E163">
@@ -3956,7 +4008,7 @@
       <c r="C164" t="s">
         <v>36</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E164">
@@ -3976,7 +4028,7 @@
       <c r="C165" t="s">
         <v>36</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E165">
@@ -3996,7 +4048,7 @@
       <c r="C166" t="s">
         <v>36</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E166">
@@ -4016,7 +4068,7 @@
       <c r="C167" t="s">
         <v>36</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E167">
@@ -4036,7 +4088,7 @@
       <c r="C168" t="s">
         <v>36</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E168">
@@ -4056,7 +4108,7 @@
       <c r="C169" t="s">
         <v>36</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E169">
@@ -4076,7 +4128,7 @@
       <c r="C170" t="s">
         <v>36</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E170">
@@ -4096,7 +4148,7 @@
       <c r="C171" t="s">
         <v>36</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="1" t="s">
         <v>121</v>
       </c>
       <c r="E171">
@@ -4116,7 +4168,7 @@
       <c r="C172" t="s">
         <v>36</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="1" t="s">
         <v>122</v>
       </c>
       <c r="E172">
@@ -4136,7 +4188,7 @@
       <c r="C173" t="s">
         <v>36</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E173">
@@ -4156,7 +4208,7 @@
       <c r="C174" t="s">
         <v>36</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="1" t="s">
         <v>124</v>
       </c>
       <c r="E174">
@@ -4176,7 +4228,7 @@
       <c r="C175" t="s">
         <v>36</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E175">
@@ -4196,7 +4248,7 @@
       <c r="C176" t="s">
         <v>36</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E176">
@@ -4216,7 +4268,7 @@
       <c r="C177" t="s">
         <v>36</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="1" t="s">
         <v>127</v>
       </c>
       <c r="E177">
@@ -4236,7 +4288,7 @@
       <c r="C178" t="s">
         <v>36</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E178">
@@ -4256,7 +4308,7 @@
       <c r="C179" t="s">
         <v>36</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="1" t="s">
         <v>129</v>
       </c>
       <c r="E179">
@@ -4276,7 +4328,7 @@
       <c r="C180" t="s">
         <v>36</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E180">
@@ -4296,7 +4348,7 @@
       <c r="C181" t="s">
         <v>36</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="1" t="s">
         <v>131</v>
       </c>
       <c r="E181">
@@ -4316,7 +4368,7 @@
       <c r="C182" t="s">
         <v>36</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E182">
@@ -4336,7 +4388,7 @@
       <c r="C183" t="s">
         <v>36</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E183">
@@ -4356,7 +4408,7 @@
       <c r="C184" t="s">
         <v>36</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E184">
@@ -4376,7 +4428,7 @@
       <c r="C185" t="s">
         <v>36</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E185">
@@ -4396,7 +4448,7 @@
       <c r="C186" t="s">
         <v>36</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E186">
@@ -4416,7 +4468,7 @@
       <c r="C187" t="s">
         <v>36</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="1" t="s">
         <v>146</v>
       </c>
       <c r="E187">
@@ -4436,7 +4488,7 @@
       <c r="C188" t="s">
         <v>36</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E188">
@@ -4456,7 +4508,7 @@
       <c r="C189" t="s">
         <v>36</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E189">
@@ -4476,7 +4528,7 @@
       <c r="C190" t="s">
         <v>36</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E190">
@@ -4496,7 +4548,7 @@
       <c r="C191" t="s">
         <v>36</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E191">
@@ -4516,7 +4568,7 @@
       <c r="C192" t="s">
         <v>36</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="1" t="s">
         <v>142</v>
       </c>
       <c r="E192">
@@ -4536,7 +4588,7 @@
       <c r="C193" t="s">
         <v>36</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E193">
@@ -4556,7 +4608,7 @@
       <c r="C194" t="s">
         <v>36</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E194">
@@ -4576,7 +4628,7 @@
       <c r="C195" t="s">
         <v>36</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="1" t="s">
         <v>100</v>
       </c>
       <c r="E195">
@@ -4596,7 +4648,7 @@
       <c r="C196" t="s">
         <v>36</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E196">
@@ -4616,7 +4668,7 @@
       <c r="C197" t="s">
         <v>36</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E197">
@@ -4636,7 +4688,7 @@
       <c r="C198" t="s">
         <v>36</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="1" t="s">
         <v>103</v>
       </c>
       <c r="E198">
@@ -4656,7 +4708,7 @@
       <c r="C199" t="s">
         <v>36</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E199">
@@ -4676,7 +4728,7 @@
       <c r="C200" t="s">
         <v>36</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E200">
@@ -4696,7 +4748,7 @@
       <c r="C201" t="s">
         <v>36</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E201">
@@ -4716,7 +4768,7 @@
       <c r="C202" t="s">
         <v>36</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="1" t="s">
         <v>107</v>
       </c>
       <c r="E202">
@@ -4736,7 +4788,7 @@
       <c r="C203" t="s">
         <v>36</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="1" t="s">
         <v>108</v>
       </c>
       <c r="E203">
@@ -4756,7 +4808,7 @@
       <c r="C204" t="s">
         <v>36</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="1" t="s">
         <v>109</v>
       </c>
       <c r="E204">
@@ -4776,7 +4828,7 @@
       <c r="C205" t="s">
         <v>36</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="1" t="s">
         <v>110</v>
       </c>
       <c r="E205">
@@ -4796,7 +4848,7 @@
       <c r="C206" t="s">
         <v>36</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="1" t="s">
         <v>111</v>
       </c>
       <c r="E206">
@@ -4816,7 +4868,7 @@
       <c r="C207" t="s">
         <v>36</v>
       </c>
-      <c r="D207">
+      <c r="D207" s="1">
         <v>86</v>
       </c>
       <c r="E207">
@@ -4836,7 +4888,7 @@
       <c r="C208" t="s">
         <v>36</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="1" t="s">
         <v>112</v>
       </c>
       <c r="E208">
@@ -4856,7 +4908,7 @@
       <c r="C209" t="s">
         <v>36</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="1" t="s">
         <v>113</v>
       </c>
       <c r="E209">
@@ -4876,7 +4928,7 @@
       <c r="C210" t="s">
         <v>36</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="1" t="s">
         <v>114</v>
       </c>
       <c r="E210">
@@ -4896,7 +4948,7 @@
       <c r="C211" t="s">
         <v>36</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E211">
@@ -4916,7 +4968,7 @@
       <c r="C212" t="s">
         <v>36</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E212">
@@ -4936,7 +4988,7 @@
       <c r="C213" t="s">
         <v>36</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D213" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E213">
@@ -4956,7 +5008,7 @@
       <c r="C214" t="s">
         <v>36</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D214" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E214">
@@ -4976,7 +5028,7 @@
       <c r="C215" t="s">
         <v>36</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E215">
@@ -4996,7 +5048,7 @@
       <c r="C216" t="s">
         <v>36</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E216">
@@ -5016,7 +5068,7 @@
       <c r="C217" t="s">
         <v>36</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="1" t="s">
         <v>121</v>
       </c>
       <c r="E217">
@@ -5036,7 +5088,7 @@
       <c r="C218" t="s">
         <v>36</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D218" s="1" t="s">
         <v>122</v>
       </c>
       <c r="E218">
@@ -5056,7 +5108,7 @@
       <c r="C219" t="s">
         <v>36</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E219">
@@ -5076,7 +5128,7 @@
       <c r="C220" t="s">
         <v>36</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="1" t="s">
         <v>124</v>
       </c>
       <c r="E220">
@@ -5096,7 +5148,7 @@
       <c r="C221" t="s">
         <v>36</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E221">
@@ -5116,7 +5168,7 @@
       <c r="C222" t="s">
         <v>36</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E222">
@@ -5136,7 +5188,7 @@
       <c r="C223" t="s">
         <v>36</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="1" t="s">
         <v>127</v>
       </c>
       <c r="E223">
@@ -5156,7 +5208,7 @@
       <c r="C224" t="s">
         <v>36</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E224">
@@ -5176,7 +5228,7 @@
       <c r="C225" t="s">
         <v>36</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D225" s="1" t="s">
         <v>129</v>
       </c>
       <c r="E225">
@@ -5196,7 +5248,7 @@
       <c r="C226" t="s">
         <v>36</v>
       </c>
-      <c r="D226" t="s">
+      <c r="D226" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E226">
@@ -5216,7 +5268,7 @@
       <c r="C227" t="s">
         <v>36</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D227" s="1" t="s">
         <v>131</v>
       </c>
       <c r="E227">
@@ -5236,7 +5288,7 @@
       <c r="C228" t="s">
         <v>36</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="1" t="s">
         <v>132</v>
       </c>
       <c r="E228">
@@ -5256,7 +5308,7 @@
       <c r="C229" t="s">
         <v>36</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E229">
@@ -5276,7 +5328,7 @@
       <c r="C230" t="s">
         <v>36</v>
       </c>
-      <c r="D230" t="s">
+      <c r="D230" s="1" t="s">
         <v>134</v>
       </c>
       <c r="E230">
@@ -5296,7 +5348,7 @@
       <c r="C231" t="s">
         <v>36</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D231" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E231">
@@ -5316,7 +5368,7 @@
       <c r="C232" t="s">
         <v>36</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D232" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E232">
@@ -5336,7 +5388,7 @@
       <c r="C233" t="s">
         <v>36</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E233">
@@ -5356,7 +5408,7 @@
       <c r="C234" t="s">
         <v>36</v>
       </c>
-      <c r="D234" t="s">
+      <c r="D234" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E234">
@@ -5376,7 +5428,7 @@
       <c r="C235" t="s">
         <v>36</v>
       </c>
-      <c r="D235" t="s">
+      <c r="D235" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E235">
@@ -5396,7 +5448,7 @@
       <c r="C236" t="s">
         <v>36</v>
       </c>
-      <c r="D236" t="s">
+      <c r="D236" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E236">
@@ -5416,7 +5468,7 @@
       <c r="C237" t="s">
         <v>36</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D237" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E237">
@@ -5436,7 +5488,7 @@
       <c r="C238" t="s">
         <v>36</v>
       </c>
-      <c r="D238" t="s">
+      <c r="D238" s="1" t="s">
         <v>142</v>
       </c>
       <c r="E238">
@@ -5456,7 +5508,7 @@
       <c r="C239" t="s">
         <v>36</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E239">
@@ -5476,7 +5528,7 @@
       <c r="C240" t="s">
         <v>36</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D240" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E240">
@@ -5496,7 +5548,7 @@
       <c r="C241" t="s">
         <v>36</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E241">
@@ -5516,7 +5568,7 @@
       <c r="C242" t="s">
         <v>36</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D242" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E242">
@@ -5536,7 +5588,7 @@
       <c r="C243" t="s">
         <v>36</v>
       </c>
-      <c r="D243" t="s">
+      <c r="D243" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E243">
@@ -5556,7 +5608,7 @@
       <c r="C244" t="s">
         <v>36</v>
       </c>
-      <c r="D244" t="s">
+      <c r="D244" s="1" t="s">
         <v>152</v>
       </c>
       <c r="E244">
@@ -5576,7 +5628,7 @@
       <c r="C245" t="s">
         <v>36</v>
       </c>
-      <c r="D245" t="s">
+      <c r="D245" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E245">
@@ -5596,7 +5648,7 @@
       <c r="C246" t="s">
         <v>36</v>
       </c>
-      <c r="D246" t="s">
+      <c r="D246" s="1" t="s">
         <v>155</v>
       </c>
       <c r="E246">
@@ -5616,7 +5668,7 @@
       <c r="C247" t="s">
         <v>36</v>
       </c>
-      <c r="D247" t="s">
+      <c r="D247" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E247">
@@ -5636,7 +5688,7 @@
       <c r="C248" t="s">
         <v>36</v>
       </c>
-      <c r="D248" t="s">
+      <c r="D248" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E248">
@@ -5656,7 +5708,7 @@
       <c r="C249" t="s">
         <v>36</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D249" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E249">
@@ -5676,7 +5728,7 @@
       <c r="C250" t="s">
         <v>36</v>
       </c>
-      <c r="D250" t="s">
+      <c r="D250" s="1" t="s">
         <v>152</v>
       </c>
       <c r="E250">
@@ -5696,7 +5748,7 @@
       <c r="C251" t="s">
         <v>36</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D251" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E251">
@@ -5716,7 +5768,7 @@
       <c r="C252" t="s">
         <v>36</v>
       </c>
-      <c r="D252" t="s">
+      <c r="D252" s="1" t="s">
         <v>155</v>
       </c>
       <c r="E252">
@@ -5736,8 +5788,8 @@
       <c r="C253" t="s">
         <v>36</v>
       </c>
-      <c r="D253" t="s">
-        <v>184</v>
+      <c r="D253" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="E253">
         <v>17</v>
@@ -5756,7 +5808,7 @@
       <c r="C254" t="s">
         <v>36</v>
       </c>
-      <c r="D254" t="s">
+      <c r="D254" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E254">
@@ -5776,8 +5828,8 @@
       <c r="C255" t="s">
         <v>36</v>
       </c>
-      <c r="D255" t="s">
-        <v>179</v>
+      <c r="D255" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="E255">
         <v>17</v>
@@ -5796,7 +5848,7 @@
       <c r="C256" t="s">
         <v>36</v>
       </c>
-      <c r="D256" t="s">
+      <c r="D256" s="1" t="s">
         <v>166</v>
       </c>
       <c r="E256">
@@ -5816,7 +5868,7 @@
       <c r="C257" t="s">
         <v>36</v>
       </c>
-      <c r="D257" t="s">
+      <c r="D257" s="1" t="s">
         <v>162</v>
       </c>
       <c r="E257">
@@ -5836,7 +5888,7 @@
       <c r="C258" t="s">
         <v>36</v>
       </c>
-      <c r="D258" t="s">
+      <c r="D258" s="1" t="s">
         <v>164</v>
       </c>
       <c r="E258">
@@ -5856,7 +5908,7 @@
       <c r="C259" t="s">
         <v>36</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D259" s="1" t="s">
         <v>175</v>
       </c>
       <c r="E259">
@@ -5876,8 +5928,8 @@
       <c r="C260" t="s">
         <v>36</v>
       </c>
-      <c r="D260" t="s">
-        <v>178</v>
+      <c r="D260" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E260">
         <v>17</v>
@@ -5896,7 +5948,7 @@
       <c r="C261" t="s">
         <v>36</v>
       </c>
-      <c r="D261" t="s">
+      <c r="D261" s="1" t="s">
         <v>173</v>
       </c>
       <c r="E261">
@@ -5916,7 +5968,7 @@
       <c r="C262" t="s">
         <v>36</v>
       </c>
-      <c r="D262" t="s">
+      <c r="D262" s="1" t="s">
         <v>156</v>
       </c>
       <c r="E262">
@@ -5936,8 +5988,8 @@
       <c r="C263" t="s">
         <v>36</v>
       </c>
-      <c r="D263" t="s">
-        <v>181</v>
+      <c r="D263" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="E263">
         <v>17</v>
@@ -5956,7 +6008,7 @@
       <c r="C264" t="s">
         <v>36</v>
       </c>
-      <c r="D264" t="s">
+      <c r="D264" s="1" t="s">
         <v>168</v>
       </c>
       <c r="E264">
@@ -5976,7 +6028,7 @@
       <c r="C265" t="s">
         <v>36</v>
       </c>
-      <c r="D265" t="s">
+      <c r="D265" s="1" t="s">
         <v>159</v>
       </c>
       <c r="E265">
@@ -5996,7 +6048,7 @@
       <c r="C266" t="s">
         <v>36</v>
       </c>
-      <c r="D266" t="s">
+      <c r="D266" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E266">
@@ -6016,7 +6068,7 @@
       <c r="C267" t="s">
         <v>36</v>
       </c>
-      <c r="D267" t="s">
+      <c r="D267" s="1" t="s">
         <v>172</v>
       </c>
       <c r="E267">
@@ -6036,8 +6088,8 @@
       <c r="C268" t="s">
         <v>36</v>
       </c>
-      <c r="D268" t="s">
-        <v>177</v>
+      <c r="D268" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="E268">
         <v>17</v>
@@ -6056,7 +6108,7 @@
       <c r="C269" t="s">
         <v>36</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D269" s="1" t="s">
         <v>171</v>
       </c>
       <c r="E269">
@@ -6076,8 +6128,8 @@
       <c r="C270" t="s">
         <v>36</v>
       </c>
-      <c r="D270" t="s">
-        <v>180</v>
+      <c r="D270" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="E270">
         <v>17</v>
@@ -6096,7 +6148,7 @@
       <c r="C271" t="s">
         <v>36</v>
       </c>
-      <c r="D271" t="s">
+      <c r="D271" s="1" t="s">
         <v>167</v>
       </c>
       <c r="E271">
@@ -6116,7 +6168,7 @@
       <c r="C272" t="s">
         <v>36</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D272" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E272">
@@ -6136,7 +6188,7 @@
       <c r="C273" t="s">
         <v>36</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D273" s="1" t="s">
         <v>165</v>
       </c>
       <c r="E273">
@@ -6156,8 +6208,8 @@
       <c r="C274" t="s">
         <v>36</v>
       </c>
-      <c r="D274" t="s">
-        <v>176</v>
+      <c r="D274" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="E274">
         <v>17</v>
@@ -6176,8 +6228,8 @@
       <c r="C275" t="s">
         <v>36</v>
       </c>
-      <c r="D275" t="s">
-        <v>178</v>
+      <c r="D275" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E275">
         <v>17</v>
@@ -6196,7 +6248,7 @@
       <c r="C276" t="s">
         <v>36</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D276" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E276">
@@ -6216,7 +6268,7 @@
       <c r="C277" t="s">
         <v>36</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D277" s="1" t="s">
         <v>158</v>
       </c>
       <c r="E277">
@@ -6236,8 +6288,8 @@
       <c r="C278" t="s">
         <v>36</v>
       </c>
-      <c r="D278" t="s">
-        <v>182</v>
+      <c r="D278" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="E278">
         <v>17</v>
@@ -6256,7 +6308,7 @@
       <c r="C279" t="s">
         <v>36</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D279" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E279">
@@ -6276,7 +6328,7 @@
       <c r="C280" t="s">
         <v>36</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E280">
@@ -6296,7 +6348,7 @@
       <c r="C281" t="s">
         <v>36</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E281">
@@ -6316,14 +6368,350 @@
       <c r="C282" t="s">
         <v>36</v>
       </c>
-      <c r="D282" t="s">
-        <v>183</v>
+      <c r="D282" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="E282">
         <v>17</v>
       </c>
       <c r="F282" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>141</v>
+      </c>
+      <c r="B283" t="s">
+        <v>148</v>
+      </c>
+      <c r="C283" t="s">
+        <v>36</v>
+      </c>
+      <c r="D283" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>142</v>
+      </c>
+      <c r="B284" t="s">
+        <v>148</v>
+      </c>
+      <c r="C284" t="s">
+        <v>36</v>
+      </c>
+      <c r="D284" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>143</v>
+      </c>
+      <c r="B285" t="s">
+        <v>148</v>
+      </c>
+      <c r="C285" t="s">
+        <v>36</v>
+      </c>
+      <c r="D285" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>144</v>
+      </c>
+      <c r="B286" t="s">
+        <v>148</v>
+      </c>
+      <c r="C286" t="s">
+        <v>36</v>
+      </c>
+      <c r="D286" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>145</v>
+      </c>
+      <c r="B287" t="s">
+        <v>148</v>
+      </c>
+      <c r="C287" t="s">
+        <v>36</v>
+      </c>
+      <c r="D287" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>146</v>
+      </c>
+      <c r="B288" t="s">
+        <v>148</v>
+      </c>
+      <c r="C288" t="s">
+        <v>36</v>
+      </c>
+      <c r="D288" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>147</v>
+      </c>
+      <c r="B289" t="s">
+        <v>148</v>
+      </c>
+      <c r="C289" t="s">
+        <v>36</v>
+      </c>
+      <c r="D289" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>148</v>
+      </c>
+      <c r="B290" t="s">
+        <v>148</v>
+      </c>
+      <c r="C290" t="s">
+        <v>36</v>
+      </c>
+      <c r="D290" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>149</v>
+      </c>
+      <c r="B291" t="s">
+        <v>148</v>
+      </c>
+      <c r="C291" t="s">
+        <v>36</v>
+      </c>
+      <c r="D291" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>150</v>
+      </c>
+      <c r="B292" t="s">
+        <v>148</v>
+      </c>
+      <c r="C292" t="s">
+        <v>36</v>
+      </c>
+      <c r="D292" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>151</v>
+      </c>
+      <c r="B293" t="s">
+        <v>148</v>
+      </c>
+      <c r="C293" t="s">
+        <v>36</v>
+      </c>
+      <c r="D293" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>152</v>
+      </c>
+      <c r="B294" t="s">
+        <v>148</v>
+      </c>
+      <c r="C294" t="s">
+        <v>36</v>
+      </c>
+      <c r="D294" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>141</v>
+      </c>
+      <c r="B295" t="s">
+        <v>41</v>
+      </c>
+      <c r="C295" t="s">
+        <v>36</v>
+      </c>
+      <c r="D295" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>142</v>
+      </c>
+      <c r="B296" t="s">
+        <v>41</v>
+      </c>
+      <c r="C296" t="s">
+        <v>36</v>
+      </c>
+      <c r="D296" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>143</v>
+      </c>
+      <c r="B297" t="s">
+        <v>41</v>
+      </c>
+      <c r="C297" t="s">
+        <v>36</v>
+      </c>
+      <c r="D297" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>144</v>
+      </c>
+      <c r="B298" t="s">
+        <v>41</v>
+      </c>
+      <c r="C298" t="s">
+        <v>36</v>
+      </c>
+      <c r="D298" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>145</v>
+      </c>
+      <c r="B299" t="s">
+        <v>41</v>
+      </c>
+      <c r="C299" t="s">
+        <v>36</v>
+      </c>
+      <c r="D299" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>146</v>
+      </c>
+      <c r="B300" t="s">
+        <v>41</v>
+      </c>
+      <c r="C300" t="s">
+        <v>36</v>
+      </c>
+      <c r="D300" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>147</v>
+      </c>
+      <c r="B301" t="s">
+        <v>41</v>
+      </c>
+      <c r="C301" t="s">
+        <v>36</v>
+      </c>
+      <c r="D301" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>148</v>
+      </c>
+      <c r="B302" t="s">
+        <v>41</v>
+      </c>
+      <c r="C302" t="s">
+        <v>36</v>
+      </c>
+      <c r="D302" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>149</v>
+      </c>
+      <c r="B303" t="s">
+        <v>41</v>
+      </c>
+      <c r="C303" t="s">
+        <v>36</v>
+      </c>
+      <c r="D303" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>150</v>
+      </c>
+      <c r="B304" t="s">
+        <v>41</v>
+      </c>
+      <c r="C304" t="s">
+        <v>36</v>
+      </c>
+      <c r="D304" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>151</v>
+      </c>
+      <c r="B305" t="s">
+        <v>41</v>
+      </c>
+      <c r="C305" t="s">
+        <v>36</v>
+      </c>
+      <c r="D305" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>152</v>
+      </c>
+      <c r="B306" t="s">
+        <v>41</v>
+      </c>
+      <c r="C306" t="s">
+        <v>36</v>
+      </c>
+      <c r="D306" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>